<commit_message>
Nopea rämpsy että voi ajaa komentoriviltä, ei tehty nyt suoria parametreja vaan otetaan kysymällä, hieman nopeuttaa ajamista
</commit_message>
<xml_diff>
--- a/Aktiviteetit/Vuosi_2025/Heinäkuu/Aktiviteetit_Heinäkuu.xlsx
+++ b/Aktiviteetit/Vuosi_2025/Heinäkuu/Aktiviteetit_Heinäkuu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,19 +483,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Night Run</t>
+          <t>Lunch Run</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.09</v>
+        <v>12</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01:01:06</t>
+          <t>01:18:08</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3666</v>
+        <v>4688</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -504,37 +504,37 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-07-07T21:57:25Z</t>
+          <t>2025-07-09T12:24:49Z</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>06:43</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>13.679424</v>
+        <v>9.752624640000001</v>
       </c>
       <c r="I2" t="n">
-        <v>138.6</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afternoon Run</t>
+          <t>Säbä</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>21.27</v>
+        <v>6.41</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02:10:07</t>
+          <t>01:38:20</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7807</v>
+        <v>5900</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -543,37 +543,37 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-07-05T16:17:54Z</t>
+          <t>2025-07-08T19:33:57Z</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>8.928640512000001</v>
+        <v>10.68604416</v>
       </c>
       <c r="I3" t="n">
-        <v>145.7</v>
+        <v>131.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vetoja</t>
+          <t>Night Run</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.06</v>
+        <v>9.09</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00:40:04</t>
+          <t>01:01:06</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2404</v>
+        <v>3666</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -582,37 +582,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-07-03T20:37:43Z</t>
+          <t>2025-07-07T21:57:25Z</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>05:41</t>
+          <t>06:43</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>10.460736</v>
+        <v>13.679424</v>
       </c>
       <c r="I4" t="n">
-        <v>153.8</v>
+        <v>138.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Morning Run</t>
+          <t>Afternoon Run</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.65</v>
+        <v>21.27</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01:11:48</t>
+          <t>02:10:07</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4308</v>
+        <v>7807</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -621,37 +621,37 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-07-02T10:27:49Z</t>
+          <t>2025-07-05T16:17:54Z</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>06:45</t>
+          <t>06:07</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>5.676156288</v>
+        <v>8.928640512000001</v>
       </c>
       <c r="I5" t="n">
-        <v>135</v>
+        <v>145.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Vetoja</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.03</v>
+        <v>7.06</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01:18:34</t>
+          <t>00:40:04</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4714</v>
+        <v>2404</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -660,57 +660,135 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-07-01T20:42:49Z</t>
+          <t>2025-07-03T20:37:43Z</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>05:41</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>8.304215040000001</v>
+        <v>10.460736</v>
       </c>
       <c r="I6" t="n">
-        <v>142.1</v>
+        <v>153.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Morning Run</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01:11:48</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4308</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-02T10:27:49Z</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>06:45</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>5.676156288</v>
+      </c>
+      <c r="I7" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Säbä</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>01:18:34</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4714</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-07-01T20:42:49Z</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>8.304215040000001</v>
+      </c>
+      <c r="I8" t="n">
+        <v>142.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Alkulämpöfutis</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B9" t="n">
         <v>1.4</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>00:12:40</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>760</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Run</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2025-07-01T20:24:46Z</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>09:03</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="H9" t="n">
         <v>9.752624640000001</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I9" t="n">
         <v>135.1</v>
       </c>
     </row>

</xml_diff>